<commit_message>
1.0.0.0.9 checkin mudanças vendas_form
</commit_message>
<xml_diff>
--- a/viapetra.xlsx
+++ b/viapetra.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\viapetra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4021DC38-DF89-4694-AF68-8DEC947F74C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4069345-9227-4028-B384-95783ECD0253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9938EB74-E494-4FFB-BA06-98C3EC4DEB5D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{9938EB74-E494-4FFB-BA06-98C3EC4DEB5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="5" r:id="rId1"/>
@@ -181,12 +181,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,9 +207,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64C61D8-8A90-4EDC-A46C-8C0CD057DB7C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,10 +594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261B3A77-0B45-4D08-8560-370BFA76C1B6}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,8 +666,21 @@
         <v>37</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -668,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91953F2-9FB4-4A3D-8170-BD5C0B73696F}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>